<commit_message>
POH-1146: Ny excel mal for tariffendringer
</commit_message>
<xml_diff>
--- a/src/main/resources/bulk-upload/sykepengerefusjon_tariffendringer_mal_v16-12-2021.xlsx
+++ b/src/main/resources/bulk-upload/sykepengerefusjon_tariffendringer_mal_v16-12-2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustav/projects/sporenstreks/src/main/resources/bulk-upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72519CAF-D53A-FF42-9D58-E097292AFFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875063C8-DAC9-594B-A8B4-0BDD7B716396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53420" yWindow="6900" windowWidth="31540" windowHeight="17480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35840" yWindow="500" windowWidth="51200" windowHeight="26600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,42 +26,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>Utvidet refusjon av sykepenger i forbindelse med koronaviruset</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Dette dokumentet er beregnet på virksomheter som har for mange ansatte til at et vanlig web-skjema er praktisk. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Du kan max legge til 5000 arbeidstakere.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Er ikke dette tilstrekkelig, må du fylle ut og laste opp i flere omganger. </t>
-    </r>
-  </si>
   <si>
     <t>Slik fylles tallene inn:</t>
   </si>
@@ -108,7 +72,13 @@
     <t>Totalbeløp som kreves refundert</t>
   </si>
   <si>
-    <t>Tariffendring</t>
+    <t>Utvidet refusjon av sykepenger i forbindelse med koronaviruset - tariffendringer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dette dokumentet er beregnet på virksomheter som har sendt krav tidligere, men som på bakgrunn av tarffendringer ønsker å sende et oppdatert krav. Legg inn ny totalbeløp, så beregner NAV differansen mellom gammelt og nytt krav.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Du kan max legge til 5000 arbeidstakere. Er ikke dette tilstrekkelig, må du fylle ut og laste opp i flere omganger. </t>
   </si>
 </sst>
 </file>
@@ -130,14 +100,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -173,6 +135,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -206,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -225,18 +194,25 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,7 +598,7 @@
   <dimension ref="A1:Q1010"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -637,17 +613,15 @@
   <sheetData>
     <row r="1" spans="1:17" ht="37" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>17</v>
+      <c r="B1" s="16"/>
+    </row>
+    <row r="3" spans="1:17" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="7"/>
@@ -665,10 +639,10 @@
       <c r="Q3" s="8"/>
     </row>
     <row r="4" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>1</v>
+      <c r="A4" s="18" t="s">
+        <v>17</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="7"/>
@@ -687,7 +661,7 @@
     </row>
     <row r="5" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="5"/>
@@ -708,22 +682,22 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="E6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="F6" s="7" t="s">
         <v>6</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>8</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
@@ -758,7 +732,7 @@
     </row>
     <row r="8" spans="1:17" s="8" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="5"/>
@@ -770,7 +744,7 @@
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="C9" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="7"/>
@@ -778,22 +752,22 @@
     </row>
     <row r="10" spans="1:17" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="D10" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="E10" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="F10" s="13" t="s">
         <v>14</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>